<commit_message>
Added DB structure test
</commit_message>
<xml_diff>
--- a/NeverEatAlone/Iteration_Documentation/Iteration_5/RequestTable.xlsx
+++ b/NeverEatAlone/Iteration_Documentation/Iteration_5/RequestTable.xlsx
@@ -162,7 +162,7 @@
     <t>Unset</t>
   </si>
   <si>
-    <t>Unset visible to a list of contacts</t>
+    <t>Set invisible to a list of contacts</t>
   </si>
 </sst>
 </file>
@@ -633,7 +633,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Added functionality for updating alias of a contact
</commit_message>
<xml_diff>
--- a/NeverEatAlone/Iteration_Documentation/Iteration_5/RequestTable.xlsx
+++ b/NeverEatAlone/Iteration_Documentation/Iteration_5/RequestTable.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="53">
   <si>
     <t>REQUEST TYPE</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Meal</t>
   </si>
   <si>
-    <t xml:space="preserve">Fetch full account information </t>
-  </si>
-  <si>
     <t>REQUEST PARAMETERS EXAMPLES</t>
   </si>
   <si>
@@ -91,9 +88,6 @@
   </si>
   <si>
     <t>Check if the username and password both match the DB</t>
-  </si>
-  <si>
-    <t>Add a contact (now adding directly)</t>
   </si>
   <si>
     <t>Fetch all contacts of a user</t>
@@ -116,31 +110,13 @@
 {username=user2, property=value,…}]</t>
   </si>
   <si>
-    <t>[{Status=Success}, 
-{username=user1, Available=YES}, 
-{username=user1, Available=NO}]</t>
-  </si>
-  <si>
     <t xml:space="preserve"> {username=user_name, password=pw} </t>
   </si>
   <si>
     <t xml:space="preserve"> {username=user_name, email=email, password=pw} </t>
   </si>
   <si>
-    <t>[{Status=Success}, {username=user_name, email=email, password=pw, Available=YES}]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> {username=user_name, property=value,...} 
-(property=Availability, email, TrueName…)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Post a meal invitation to recipients </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> {recipientlist={user1,user2}, poster=user0, postType="MEAL", postID=10, (meal data)} </t>
-  </si>
-  <si>
-    <t>[{Status=Success}, {poster=user0, postType="MEAL", postID=10, (meal data)}]</t>
   </si>
   <si>
     <t>Visibility</t>
@@ -163,13 +139,70 @@
   </si>
   <si>
     <t>Set invisible to a list of contacts</t>
+  </si>
+  <si>
+    <t>{username=user_name, contactname=contact, alias=abc}</t>
+  </si>
+  <si>
+    <t>Update the alias of a contact</t>
+  </si>
+  <si>
+    <t>{username=user_name, contactname=contact}</t>
+  </si>
+  <si>
+    <t>[{Status=Success}, {Username=user_name,...}]</t>
+  </si>
+  <si>
+    <t>[{Status=Success}, {alias=abc}]</t>
+  </si>
+  <si>
+    <t>[{Status=Success}, 
+{username=user_name, …}]</t>
+  </si>
+  <si>
+    <t>Delete a contact</t>
+  </si>
+  <si>
+    <t>[{Status=Success}, {username=user_name, email=email, password=pw}]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {username=user_name, property=value,...} 
+(property=email, TrueName…)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Fetch full account information. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="20"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Note: redundant method. </t>
+    </r>
+  </si>
+  <si>
+    <t>Add a contact (adding both directions)</t>
+  </si>
+  <si>
+    <t>[{Status=Success}, {username=user1}, 
+{username=user2}]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {recipientlist={user1,user2}, poster=user0, postType="MEAL", postID=10,... (meal data)} </t>
+  </si>
+  <si>
+    <t>[{Status=Success}, {poster=user0, postType="MEAL", postID=10,... (meal data)}]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="20"/>
       <color theme="1"/>
@@ -193,6 +226,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -254,9 +307,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -630,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" x14ac:dyDescent="0"/>
@@ -653,10 +714,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
         <v>17</v>
-      </c>
-      <c r="D1" t="s">
-        <v>18</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -670,13 +731,13 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="50">
@@ -687,13 +748,13 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="22" customHeight="1">
@@ -704,13 +765,13 @@
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="53" customHeight="1">
@@ -721,30 +782,30 @@
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="50">
-      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="2" customFormat="1" ht="50">
+      <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
+      <c r="C6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="50">
@@ -755,13 +816,13 @@
         <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="50">
@@ -772,16 +833,16 @@
         <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="75">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="50">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -789,38 +850,38 @@
         <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="56" customHeight="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="50">
       <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B10" t="s">
+      <c r="D10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="56" customHeight="1">
+    </row>
+    <row r="11" spans="1:5" ht="50">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>41</v>
@@ -832,21 +893,55 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="50">
-      <c r="A12" t="s">
+    <row r="12" spans="1:5" s="4" customFormat="1" ht="56" customHeight="1">
+      <c r="A12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="4" customFormat="1" ht="56" customHeight="1">
+      <c r="A13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="50">
+      <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B14" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" t="s">
-        <v>36</v>
+      <c r="C14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified GetAllContacts() and resolved email uniqueness issue
</commit_message>
<xml_diff>
--- a/NeverEatAlone/Iteration_Documentation/Iteration_5/RequestTable.xlsx
+++ b/NeverEatAlone/Iteration_Documentation/Iteration_5/RequestTable.xlsx
@@ -188,14 +188,13 @@
     <t>Add a contact (adding both directions)</t>
   </si>
   <si>
-    <t>[{Status=Success}, {username=user1}, 
-{username=user2}]</t>
-  </si>
-  <si>
     <t xml:space="preserve"> {recipientlist={user1,user2}, poster=user0, postType="MEAL", postID=10,... (meal data)} </t>
   </si>
   <si>
     <t>[{Status=Success}, {poster=user0, postType="MEAL", postID=10,... (meal data)}]</t>
+  </si>
+  <si>
+    <t>[{Status=Success}, {Username=user_1, alias=abc},{Username=user_2, alias=blabla},…]</t>
   </si>
 </sst>
 </file>
@@ -693,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" x14ac:dyDescent="0"/>
@@ -853,7 +852,7 @@
         <v>24</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E9" t="s">
         <v>23</v>
@@ -935,10 +934,10 @@
         <v>15</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="E14" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
small modification of RequestTable
</commit_message>
<xml_diff>
--- a/NeverEatAlone/Iteration_Documentation/Iteration_5/RequestTable.xlsx
+++ b/NeverEatAlone/Iteration_Documentation/Iteration_5/RequestTable.xlsx
@@ -106,10 +106,6 @@
     <t xml:space="preserve"> {username=user1, contactusername=user2} </t>
   </si>
   <si>
-    <t>[{Status=Success},
-{username=user2, property=value,…}]</t>
-  </si>
-  <si>
     <t xml:space="preserve"> {username=user_name, password=pw} </t>
   </si>
   <si>
@@ -185,16 +181,20 @@
     </r>
   </si>
   <si>
-    <t>Add a contact (adding both directions)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> {recipientlist={user1,user2}, poster=user0, postType="MEAL", postID=10,... (meal data)} </t>
   </si>
   <si>
     <t>[{Status=Success}, {poster=user0, postType="MEAL", postID=10,... (meal data)}]</t>
   </si>
   <si>
-    <t>[{Status=Success}, {Username=user_1, alias=abc},{Username=user_2, alias=blabla},…]</t>
+    <t>[{Status=Success},
+{username=user2, alias=}]</t>
+  </si>
+  <si>
+    <t>[{Status=Success}, {Username=user_1, alias=},{Username=user_2, alias=blabla},…]</t>
+  </si>
+  <si>
+    <t>Add a contact (adding both directions), and alias=""</t>
   </si>
 </sst>
 </file>
@@ -692,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" x14ac:dyDescent="0"/>
@@ -730,10 +730,10 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
         <v>18</v>
@@ -781,7 +781,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>25</v>
@@ -804,7 +804,7 @@
         <v>25</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="50">
@@ -815,7 +815,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>25</v>
@@ -835,10 +835,10 @@
         <v>27</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="E8" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="50">
@@ -852,7 +852,7 @@
         <v>24</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E9" t="s">
         <v>23</v>
@@ -866,13 +866,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" t="s">
         <v>39</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="50">
@@ -883,47 +883,47 @@
         <v>6</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="E11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="4" customFormat="1" ht="56" customHeight="1">
       <c r="A12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="C12" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="D12" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="4" customFormat="1" ht="56" customHeight="1">
       <c r="A13" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="50">
@@ -934,13 +934,13 @@
         <v>15</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added functionality for deleting contact and rejecting friend request
</commit_message>
<xml_diff>
--- a/NeverEatAlone/Iteration_Documentation/Iteration_5/RequestTable.xlsx
+++ b/NeverEatAlone/Iteration_Documentation/Iteration_5/RequestTable.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="80" windowWidth="31860" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -112,9 +112,6 @@
     <t>{username=user_name, contactname=contact}</t>
   </si>
   <si>
-    <t>[{Status=Success}, {Username=user_name,...}]</t>
-  </si>
-  <si>
     <t>[{Status=Success}, {alias=abc}]</t>
   </si>
   <si>
@@ -208,6 +205,9 @@
   </si>
   <si>
     <t>Get all contacts that are visible to this user</t>
+  </si>
+  <si>
+    <t>[{Status=Success},{username=user_name},{contactusername=contact}]</t>
   </si>
 </sst>
 </file>
@@ -708,7 +708,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" x14ac:dyDescent="0"/>
@@ -742,13 +742,13 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -759,7 +759,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>16</v>
@@ -776,7 +776,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>16</v>
@@ -793,10 +793,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>17</v>
@@ -810,7 +810,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>16</v>
@@ -819,7 +819,7 @@
         <v>17</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="50">
@@ -827,7 +827,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>20</v>
@@ -844,16 +844,16 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="50">
@@ -861,13 +861,13 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E9" t="s">
         <v>15</v>
@@ -878,13 +878,13 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" t="s">
         <v>28</v>
@@ -895,16 +895,16 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="4" customFormat="1" ht="56" customHeight="1">
@@ -912,13 +912,13 @@
         <v>23</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>49</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>50</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>25</v>
@@ -929,13 +929,13 @@
         <v>23</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>26</v>
@@ -946,16 +946,16 @@
         <v>23</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="4" customFormat="1" ht="56" customHeight="1">
@@ -963,16 +963,16 @@
         <v>23</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="50">
@@ -983,10 +983,10 @@
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="E16" t="s">
         <v>22</v>

</xml_diff>